<commit_message>
added main method file to suite, updated test cases for risk assessment
</commit_message>
<xml_diff>
--- a/qa/src/main/resources/TestDataBreathe.xlsx
+++ b/qa/src/main/resources/TestDataBreathe.xlsx
@@ -1,13 +1,8 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\QA_Breathe_git\breathe\qa\src\main\resources\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
+  <workbookPr/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" activeTab="2"/>
   </bookViews>
@@ -17,7 +12,7 @@
     <sheet name="RiskAssessment" sheetId="2" r:id="rId3"/>
     <sheet name="RiskScenarios" sheetId="3" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="145621"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -131,9 +126,6 @@
     <t>ID</t>
   </si>
   <si>
-    <t>In the past month, how frequently did your asthma keep you from getting as much done at work, school or at home? Potential answers (user can select one and only one</t>
-  </si>
-  <si>
     <t>In the past month, how many instances of shortness of breath (SOB) have you had? Potential answers (user can select one and only one):</t>
   </si>
   <si>
@@ -201,6 +193,9 @@
   </si>
   <si>
     <t>Smoke</t>
+  </si>
+  <si>
+    <t>In the past month, how frequently did your asthma keep you from getting as much done at work, school or at home? Potential answers (user can select one and only one)</t>
   </si>
 </sst>
 </file>
@@ -537,7 +532,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -605,7 +600,7 @@
   <sheetData>
     <row r="1" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B1" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C1" t="s">
         <v>23</v>
@@ -619,7 +614,7 @@
     </row>
     <row r="2" spans="2:5" ht="25.5" x14ac:dyDescent="0.25">
       <c r="B2" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C2" t="s">
         <v>25</v>
@@ -641,7 +636,7 @@
   <dimension ref="A1:R4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -672,31 +667,31 @@
         <v>7</v>
       </c>
       <c r="H1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="I1" t="s">
         <v>8</v>
       </c>
       <c r="J1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="K1" t="s">
         <v>9</v>
       </c>
       <c r="L1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="M1" t="s">
         <v>10</v>
       </c>
       <c r="N1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="O1" t="s">
         <v>11</v>
       </c>
       <c r="P1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="Q1" t="s">
         <v>12</v>
@@ -710,7 +705,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>34</v>
+        <v>57</v>
       </c>
       <c r="C2" t="s">
         <v>0</v>
@@ -725,31 +720,31 @@
         <v>0</v>
       </c>
       <c r="G2" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="H2">
+        <v>0</v>
+      </c>
+      <c r="I2" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="H2">
-        <v>0</v>
-      </c>
-      <c r="I2" s="4" t="s">
+      <c r="J2">
+        <v>0</v>
+      </c>
+      <c r="K2" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="J2">
-        <v>0</v>
-      </c>
-      <c r="K2" s="4" t="s">
+      <c r="L2">
+        <v>0</v>
+      </c>
+      <c r="M2" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="L2">
-        <v>0</v>
-      </c>
-      <c r="M2" s="4" t="s">
+      <c r="N2">
+        <v>0</v>
+      </c>
+      <c r="O2" s="4" t="s">
         <v>47</v>
-      </c>
-      <c r="N2">
-        <v>0</v>
-      </c>
-      <c r="O2" s="4" t="s">
-        <v>48</v>
       </c>
       <c r="P2">
         <v>0</v>
@@ -760,7 +755,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C3" t="s">
         <v>0</v>
@@ -775,31 +770,31 @@
         <v>0</v>
       </c>
       <c r="G3" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="H3">
+        <v>0</v>
+      </c>
+      <c r="I3" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="H3">
-        <v>0</v>
-      </c>
-      <c r="I3" s="4" t="s">
+      <c r="J3">
+        <v>0</v>
+      </c>
+      <c r="K3" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="J3">
-        <v>0</v>
-      </c>
-      <c r="K3" s="4" t="s">
+      <c r="L3">
+        <v>0</v>
+      </c>
+      <c r="M3" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="L3">
-        <v>0</v>
-      </c>
-      <c r="M3" s="4" t="s">
-        <v>52</v>
-      </c>
       <c r="N3">
         <v>0</v>
       </c>
       <c r="O3" s="4" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="P3">
         <v>0</v>
@@ -810,7 +805,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C4" t="s">
         <v>0</v>
@@ -825,31 +820,31 @@
         <v>0</v>
       </c>
       <c r="G4" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="H4">
+        <v>0</v>
+      </c>
+      <c r="I4" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="H4">
-        <v>0</v>
-      </c>
-      <c r="I4" s="4" t="s">
+      <c r="J4">
+        <v>0</v>
+      </c>
+      <c r="K4" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="J4">
-        <v>0</v>
-      </c>
-      <c r="K4" s="4" t="s">
+      <c r="L4">
+        <v>0</v>
+      </c>
+      <c r="M4" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="L4">
-        <v>0</v>
-      </c>
-      <c r="M4" s="4" t="s">
+      <c r="N4">
+        <v>0</v>
+      </c>
+      <c r="O4" s="4" t="s">
         <v>56</v>
-      </c>
-      <c r="N4">
-        <v>0</v>
-      </c>
-      <c r="O4" s="4" t="s">
-        <v>57</v>
       </c>
       <c r="P4">
         <v>0</v>

</xml_diff>

<commit_message>
added and updated more test cases
</commit_message>
<xml_diff>
--- a/qa/src/main/resources/TestDataBreathe.xlsx
+++ b/qa/src/main/resources/TestDataBreathe.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="UserData" sheetId="4" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="58">
   <si>
     <t>y</t>
   </si>
@@ -532,7 +532,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -635,7 +635,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
@@ -860,8 +860,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -921,8 +921,8 @@
       <c r="A4">
         <v>3</v>
       </c>
-      <c r="B4">
-        <v>1</v>
+      <c r="B4" t="s">
+        <v>16</v>
       </c>
       <c r="C4">
         <v>1</v>

</xml_diff>

<commit_message>
added teststarthealthriskassessment class and updated test cases
</commit_message>
<xml_diff>
--- a/qa/src/main/resources/TestDataBreathe.xlsx
+++ b/qa/src/main/resources/TestDataBreathe.xlsx
@@ -1,15 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\QA_Breathe\breathe\qa\src\main\resources\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="UserData" sheetId="4" r:id="rId1"/>
@@ -17,7 +12,7 @@
     <sheet name="RiskAssessment" sheetId="2" r:id="rId3"/>
     <sheet name="RiskScenarios" sheetId="3" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="145621"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -27,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="65">
   <si>
     <t>y</t>
   </si>
@@ -216,6 +211,12 @@
   </si>
   <si>
     <t>Riskc5</t>
+  </si>
+  <si>
+    <t>n</t>
+  </si>
+  <si>
+    <t>status</t>
   </si>
 </sst>
 </file>
@@ -552,7 +553,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -655,7 +656,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:W4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="O4" sqref="O4"/>
     </sheetView>
   </sheetViews>
@@ -954,10 +955,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E8"/>
+  <dimension ref="A1:E9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -980,121 +981,138 @@
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2">
-        <v>1</v>
-      </c>
-      <c r="B2">
-        <v>3</v>
-      </c>
-      <c r="C2">
-        <v>2</v>
-      </c>
-      <c r="D2">
-        <v>3</v>
-      </c>
-      <c r="E2">
-        <v>3</v>
+      <c r="A2" t="s">
+        <v>64</v>
+      </c>
+      <c r="B2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E2" t="s">
+        <v>63</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="B3">
+        <v>3</v>
+      </c>
+      <c r="C3">
         <v>2</v>
       </c>
-      <c r="B3">
-        <v>2</v>
-      </c>
-      <c r="C3">
+      <c r="D3">
         <v>3</v>
       </c>
-      <c r="D3">
-        <v>2</v>
-      </c>
       <c r="E3">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4">
+        <v>2</v>
+      </c>
+      <c r="B4">
+        <v>2</v>
+      </c>
+      <c r="C4">
         <v>3</v>
       </c>
-      <c r="B4">
-        <v>1</v>
-      </c>
-      <c r="C4">
-        <v>1</v>
-      </c>
       <c r="D4">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E4">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5">
-        <v>4</v>
-      </c>
-      <c r="B5" t="s">
-        <v>16</v>
-      </c>
-      <c r="C5" t="s">
-        <v>16</v>
-      </c>
-      <c r="D5" t="s">
-        <v>16</v>
-      </c>
-      <c r="E5" t="s">
-        <v>16</v>
+        <v>3</v>
+      </c>
+      <c r="B5">
+        <v>1</v>
+      </c>
+      <c r="C5">
+        <v>1</v>
+      </c>
+      <c r="D5">
+        <v>1</v>
+      </c>
+      <c r="E5">
+        <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6">
-        <v>5</v>
-      </c>
-      <c r="B6">
-        <v>2</v>
-      </c>
-      <c r="C6">
-        <v>2</v>
-      </c>
-      <c r="D6">
-        <v>2</v>
-      </c>
-      <c r="E6">
-        <v>0</v>
+        <v>4</v>
+      </c>
+      <c r="B6" t="s">
+        <v>16</v>
+      </c>
+      <c r="C6" t="s">
+        <v>16</v>
+      </c>
+      <c r="D6" t="s">
+        <v>16</v>
+      </c>
+      <c r="E6" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7">
-        <v>6</v>
-      </c>
-      <c r="B7" t="s">
-        <v>17</v>
-      </c>
-      <c r="C7" t="s">
-        <v>17</v>
+        <v>5</v>
+      </c>
+      <c r="B7">
+        <v>2</v>
+      </c>
+      <c r="C7">
+        <v>2</v>
       </c>
       <c r="D7">
+        <v>2</v>
+      </c>
+      <c r="E7">
         <v>0</v>
-      </c>
-      <c r="E7" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8">
+        <v>6</v>
+      </c>
+      <c r="B8" t="s">
+        <v>17</v>
+      </c>
+      <c r="C8" t="s">
+        <v>17</v>
+      </c>
+      <c r="D8">
+        <v>0</v>
+      </c>
+      <c r="E8" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9">
         <v>7</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B9" t="s">
         <v>18</v>
       </c>
-      <c r="C8" t="s">
+      <c r="C9" t="s">
         <v>18</v>
       </c>
-      <c r="D8" t="s">
+      <c r="D9" t="s">
         <v>18</v>
       </c>
-      <c r="E8" t="s">
+      <c r="E9" t="s">
         <v>18</v>
       </c>
     </row>

</xml_diff>

<commit_message>
made scenario working from excel, updated main class, TestHealthAssessmentQuestions
</commit_message>
<xml_diff>
--- a/qa/src/main/resources/TestDataBreathe.xlsx
+++ b/qa/src/main/resources/TestDataBreathe.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="60">
   <si>
     <t>y</t>
   </si>
@@ -196,21 +196,6 @@
   </si>
   <si>
     <t>In the past month, how frequently did your asthma keep you from getting as much done at work, school or at home? Potential answers (user can select one and only one)</t>
-  </si>
-  <si>
-    <t>Riskc1</t>
-  </si>
-  <si>
-    <t>Riskc2</t>
-  </si>
-  <si>
-    <t>Riskc3</t>
-  </si>
-  <si>
-    <t>Riskc4</t>
-  </si>
-  <si>
-    <t>Riskc5</t>
   </si>
   <si>
     <t>n</t>
@@ -268,7 +253,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -280,6 +265,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -654,19 +640,18 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:W4"/>
+  <dimension ref="A1:R4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="O4" sqref="O4"/>
+      <selection activeCell="S1" sqref="S1:W1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="22.28515625" style="2" customWidth="1"/>
-    <col min="19" max="20" width="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>33</v>
       </c>
@@ -721,23 +706,8 @@
       <c r="R1" t="s">
         <v>15</v>
       </c>
-      <c r="S1" t="s">
-        <v>58</v>
-      </c>
-      <c r="T1" t="s">
-        <v>59</v>
-      </c>
-      <c r="U1" t="s">
-        <v>60</v>
-      </c>
-      <c r="V1" t="s">
-        <v>61</v>
-      </c>
-      <c r="W1" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="2" spans="1:23" ht="114.75" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:18" ht="114.75" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -786,28 +756,8 @@
       <c r="P2">
         <v>1</v>
       </c>
-      <c r="S2">
-        <f>F2*(H2)</f>
-        <v>1</v>
-      </c>
-      <c r="T2">
-        <f>F2*(J2)</f>
-        <v>1</v>
-      </c>
-      <c r="U2">
-        <f>F2*(L2)</f>
-        <v>1</v>
-      </c>
-      <c r="V2">
-        <f>F2*(N2)</f>
-        <v>1</v>
-      </c>
-      <c r="W2">
-        <f>F2*(P2)</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:23" ht="102" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:18" ht="102" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -856,28 +806,8 @@
       <c r="P3">
         <v>1</v>
       </c>
-      <c r="S3">
-        <f>F3*(H3)</f>
-        <v>1</v>
-      </c>
-      <c r="T3">
-        <f>F3*(J3)</f>
-        <v>1</v>
-      </c>
-      <c r="U3">
-        <f>F3*(L3)</f>
-        <v>1</v>
-      </c>
-      <c r="V3">
-        <f>F3*(N3)</f>
-        <v>1</v>
-      </c>
-      <c r="W3">
-        <f>F3*(P3)</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:23" ht="76.5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="4" spans="1:18" ht="76.5" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -924,26 +854,6 @@
         <v>56</v>
       </c>
       <c r="P4">
-        <v>1</v>
-      </c>
-      <c r="S4">
-        <f>F4*(H4)</f>
-        <v>1</v>
-      </c>
-      <c r="T4">
-        <f>F4*(J4)</f>
-        <v>1</v>
-      </c>
-      <c r="U4">
-        <f>F4*(L4)</f>
-        <v>1</v>
-      </c>
-      <c r="V4">
-        <f>F4*(N4)</f>
-        <v>1</v>
-      </c>
-      <c r="W4">
-        <f>F4*(P4)</f>
         <v>1</v>
       </c>
     </row>
@@ -958,7 +868,7 @@
   <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -982,7 +892,7 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="B2" t="s">
         <v>6</v>
@@ -994,23 +904,23 @@
         <v>6</v>
       </c>
       <c r="E2" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>1</v>
       </c>
-      <c r="B3">
+      <c r="B3" s="5">
         <v>3</v>
       </c>
-      <c r="C3">
+      <c r="C3" s="5">
         <v>2</v>
       </c>
-      <c r="D3">
+      <c r="D3" s="5">
         <v>3</v>
       </c>
-      <c r="E3">
+      <c r="E3" s="5">
         <v>3</v>
       </c>
     </row>
@@ -1018,16 +928,16 @@
       <c r="A4">
         <v>2</v>
       </c>
-      <c r="B4">
+      <c r="B4" s="5">
         <v>2</v>
       </c>
-      <c r="C4">
+      <c r="C4" s="5">
         <v>3</v>
       </c>
-      <c r="D4">
+      <c r="D4" s="5">
         <v>2</v>
       </c>
-      <c r="E4">
+      <c r="E4" s="5">
         <v>2</v>
       </c>
     </row>
@@ -1035,16 +945,16 @@
       <c r="A5">
         <v>3</v>
       </c>
-      <c r="B5">
-        <v>1</v>
-      </c>
-      <c r="C5">
-        <v>1</v>
-      </c>
-      <c r="D5">
-        <v>1</v>
-      </c>
-      <c r="E5">
+      <c r="B5" s="5">
+        <v>1</v>
+      </c>
+      <c r="C5" s="5">
+        <v>1</v>
+      </c>
+      <c r="D5" s="5">
+        <v>1</v>
+      </c>
+      <c r="E5" s="5">
         <v>0</v>
       </c>
     </row>
@@ -1052,16 +962,16 @@
       <c r="A6">
         <v>4</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C6" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="D6" t="s">
+      <c r="D6" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="E6" t="s">
+      <c r="E6" s="5" t="s">
         <v>16</v>
       </c>
     </row>
@@ -1069,16 +979,16 @@
       <c r="A7">
         <v>5</v>
       </c>
-      <c r="B7">
+      <c r="B7" s="5">
         <v>2</v>
       </c>
-      <c r="C7">
+      <c r="C7" s="5">
         <v>2</v>
       </c>
-      <c r="D7">
+      <c r="D7" s="5">
         <v>2</v>
       </c>
-      <c r="E7">
+      <c r="E7" s="5">
         <v>0</v>
       </c>
     </row>
@@ -1086,16 +996,16 @@
       <c r="A8">
         <v>6</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B8" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="C8" t="s">
+      <c r="C8" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="D8">
+      <c r="D8" s="5">
         <v>0</v>
       </c>
-      <c r="E8" t="s">
+      <c r="E8" s="5" t="s">
         <v>17</v>
       </c>
     </row>
@@ -1103,20 +1013,21 @@
       <c r="A9">
         <v>7</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B9" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="C9" t="s">
+      <c r="C9" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="D9" t="s">
+      <c r="D9" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="E9" t="s">
+      <c r="E9" s="5" t="s">
         <v>18</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
made scenario working from excel for checkbox based multiple choice question
</commit_message>
<xml_diff>
--- a/qa/src/main/resources/TestDataBreathe.xlsx
+++ b/qa/src/main/resources/TestDataBreathe.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="61">
   <si>
     <t>y</t>
   </si>
@@ -202,6 +202,9 @@
   </si>
   <si>
     <t>status</t>
+  </si>
+  <si>
+    <t>1,3</t>
   </si>
 </sst>
 </file>
@@ -539,7 +542,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -868,7 +871,7 @@
   <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -945,8 +948,8 @@
       <c r="A5">
         <v>3</v>
       </c>
-      <c r="B5" s="5">
-        <v>1</v>
+      <c r="B5" s="5" t="s">
+        <v>60</v>
       </c>
       <c r="C5" s="5">
         <v>1</v>

</xml_diff>

<commit_message>
Change looping for risk calculation
</commit_message>
<xml_diff>
--- a/qa/src/main/resources/TestDataBreathe.xlsx
+++ b/qa/src/main/resources/TestDataBreathe.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\QA_Breathe\breathe\qa\src\main\resources\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="UserData" sheetId="4" r:id="rId1"/>
@@ -147,9 +152,6 @@
     <t>cweight5</t>
   </si>
   <si>
-    <t>Questionaire Title</t>
-  </si>
-  <si>
     <t>Asthma Questionnaire for Beginners</t>
   </si>
   <si>
@@ -205,6 +207,9 @@
   </si>
   <si>
     <t>1,3</t>
+  </si>
+  <si>
+    <t>QuestionaireTitle</t>
   </si>
 </sst>
 </file>
@@ -542,7 +547,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -597,8 +602,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:E2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H14" sqref="H14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -610,7 +615,7 @@
   <sheetData>
     <row r="1" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B1" s="2" t="s">
-        <v>41</v>
+        <v>60</v>
       </c>
       <c r="C1" t="s">
         <v>23</v>
@@ -624,7 +629,7 @@
     </row>
     <row r="2" spans="2:5" ht="25.5" x14ac:dyDescent="0.25">
       <c r="B2" s="3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C2" t="s">
         <v>25</v>
@@ -715,7 +720,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C2" t="s">
         <v>0</v>
@@ -730,31 +735,31 @@
         <v>1</v>
       </c>
       <c r="G2" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="H2">
+        <v>1</v>
+      </c>
+      <c r="I2" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="H2">
-        <v>1</v>
-      </c>
-      <c r="I2" s="4" t="s">
+      <c r="J2">
+        <v>1</v>
+      </c>
+      <c r="K2" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="J2">
-        <v>1</v>
-      </c>
-      <c r="K2" s="4" t="s">
+      <c r="L2">
+        <v>1</v>
+      </c>
+      <c r="M2" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="L2">
-        <v>1</v>
-      </c>
-      <c r="M2" s="4" t="s">
+      <c r="N2">
+        <v>1</v>
+      </c>
+      <c r="O2" s="4" t="s">
         <v>46</v>
-      </c>
-      <c r="N2">
-        <v>1</v>
-      </c>
-      <c r="O2" s="4" t="s">
-        <v>47</v>
       </c>
       <c r="P2">
         <v>1</v>
@@ -780,31 +785,31 @@
         <v>1</v>
       </c>
       <c r="G3" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="H3">
+        <v>1</v>
+      </c>
+      <c r="I3" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="H3">
-        <v>1</v>
-      </c>
-      <c r="I3" s="4" t="s">
+      <c r="J3">
+        <v>1</v>
+      </c>
+      <c r="K3" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="J3">
-        <v>1</v>
-      </c>
-      <c r="K3" s="4" t="s">
+      <c r="L3">
+        <v>1</v>
+      </c>
+      <c r="M3" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="L3">
-        <v>1</v>
-      </c>
-      <c r="M3" s="4" t="s">
-        <v>51</v>
-      </c>
       <c r="N3">
         <v>1</v>
       </c>
       <c r="O3" s="4" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="P3">
         <v>1</v>
@@ -830,31 +835,31 @@
         <v>1</v>
       </c>
       <c r="G4" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="H4">
+        <v>1</v>
+      </c>
+      <c r="I4" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="H4">
-        <v>1</v>
-      </c>
-      <c r="I4" s="4" t="s">
+      <c r="J4">
+        <v>1</v>
+      </c>
+      <c r="K4" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="J4">
-        <v>1</v>
-      </c>
-      <c r="K4" s="4" t="s">
+      <c r="L4">
+        <v>1</v>
+      </c>
+      <c r="M4" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="L4">
-        <v>1</v>
-      </c>
-      <c r="M4" s="4" t="s">
+      <c r="N4">
+        <v>1</v>
+      </c>
+      <c r="O4" s="4" t="s">
         <v>55</v>
-      </c>
-      <c r="N4">
-        <v>1</v>
-      </c>
-      <c r="O4" s="4" t="s">
-        <v>56</v>
       </c>
       <c r="P4">
         <v>1</v>
@@ -870,7 +875,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
@@ -895,7 +900,7 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B2" t="s">
         <v>6</v>
@@ -907,7 +912,7 @@
         <v>6</v>
       </c>
       <c r="E2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
@@ -949,7 +954,7 @@
         <v>3</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C5" s="5">
         <v>1</v>

</xml_diff>

<commit_message>
Unchecking logic for score calculation added
</commit_message>
<xml_diff>
--- a/qa/src/main/resources/TestDataBreathe.xlsx
+++ b/qa/src/main/resources/TestDataBreathe.xlsx
@@ -654,7 +654,7 @@
   <dimension ref="A1:R4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J2" sqref="J2"/>
+      <selection activeCell="P2" sqref="P2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -879,7 +879,7 @@
   <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J6" sqref="J6"/>
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>